<commit_message>
started created lab for OOP
</commit_message>
<xml_diff>
--- a/Semester3/ASD/lab/ResultLab1.xlsx
+++ b/Semester3/ASD/lab/ResultLab1.xlsx
@@ -573,7 +573,7 @@
   <dimension ref="A1:E68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
@@ -621,12 +621,12 @@
         <v>1</v>
       </c>
       <c r="B3" s="10" t="n">
-        <v>50</v>
+        <v>50000</v>
       </c>
       <c r="C3" s="11" t="n"/>
       <c r="D3" s="14" t="inlineStr">
         <is>
-          <t>0.00008</t>
+          <t>94.06593</t>
         </is>
       </c>
       <c r="E3" s="6" t="n"/>
@@ -636,12 +636,12 @@
         <v>2</v>
       </c>
       <c r="B4" s="10" t="n">
-        <v>100</v>
+        <v>100000</v>
       </c>
       <c r="C4" s="11" t="n"/>
       <c r="D4" s="11" t="inlineStr">
         <is>
-          <t>0.00030</t>
+          <t>381.88609</t>
         </is>
       </c>
       <c r="E4" s="6" t="n"/>
@@ -654,7 +654,11 @@
         <v>150000</v>
       </c>
       <c r="C5" s="11" t="n"/>
-      <c r="D5" s="11" t="n"/>
+      <c r="D5" s="11" t="inlineStr">
+        <is>
+          <t>869.28647</t>
+        </is>
+      </c>
       <c r="E5" s="6" t="n"/>
     </row>
     <row r="6">
@@ -665,7 +669,11 @@
         <v>200000</v>
       </c>
       <c r="C6" s="11" t="n"/>
-      <c r="D6" s="11" t="n"/>
+      <c r="D6" s="11" t="inlineStr">
+        <is>
+          <t>1564.29378</t>
+        </is>
+      </c>
       <c r="E6" s="6" t="n"/>
     </row>
     <row r="7">
@@ -676,7 +684,11 @@
         <v>250000</v>
       </c>
       <c r="C7" s="11" t="n"/>
-      <c r="D7" s="11" t="n"/>
+      <c r="D7" s="11" t="inlineStr">
+        <is>
+          <t>2527.58961</t>
+        </is>
+      </c>
       <c r="E7" s="6" t="n"/>
     </row>
     <row r="8">
@@ -687,7 +699,11 @@
         <v>300000</v>
       </c>
       <c r="C8" s="11" t="n"/>
-      <c r="D8" s="11" t="n"/>
+      <c r="D8" s="11" t="inlineStr">
+        <is>
+          <t>3520.05186</t>
+        </is>
+      </c>
       <c r="E8" s="6" t="n"/>
     </row>
     <row r="9">
@@ -698,7 +714,11 @@
         <v>350000</v>
       </c>
       <c r="C9" s="11" t="n"/>
-      <c r="D9" s="11" t="n"/>
+      <c r="D9" s="11" t="inlineStr">
+        <is>
+          <t>4715.42362</t>
+        </is>
+      </c>
       <c r="E9" s="6" t="n"/>
     </row>
     <row r="10">
@@ -709,7 +729,11 @@
         <v>400000</v>
       </c>
       <c r="C10" s="11" t="n"/>
-      <c r="D10" s="11" t="n"/>
+      <c r="D10" s="11" t="inlineStr">
+        <is>
+          <t>7078.99730</t>
+        </is>
+      </c>
       <c r="E10" s="6" t="n"/>
     </row>
     <row r="11">
@@ -720,7 +744,11 @@
         <v>450000</v>
       </c>
       <c r="C11" s="11" t="n"/>
-      <c r="D11" s="11" t="n"/>
+      <c r="D11" s="11" t="inlineStr">
+        <is>
+          <t>9364.29803</t>
+        </is>
+      </c>
       <c r="E11" s="6" t="n"/>
     </row>
     <row r="12">
@@ -731,7 +759,11 @@
         <v>500000</v>
       </c>
       <c r="C12" s="11" t="n"/>
-      <c r="D12" s="11" t="n"/>
+      <c r="D12" s="11" t="inlineStr">
+        <is>
+          <t>11663.87637</t>
+        </is>
+      </c>
       <c r="E12" s="6" t="n"/>
     </row>
     <row r="13">
@@ -742,7 +774,11 @@
         <v>550000</v>
       </c>
       <c r="C13" s="11" t="n"/>
-      <c r="D13" s="11" t="n"/>
+      <c r="D13" s="11" t="inlineStr">
+        <is>
+          <t>13622.29164</t>
+        </is>
+      </c>
       <c r="E13" s="6" t="n"/>
     </row>
     <row r="14">
@@ -753,7 +789,11 @@
         <v>600000</v>
       </c>
       <c r="C14" s="11" t="n"/>
-      <c r="D14" s="11" t="n"/>
+      <c r="D14" s="11" t="inlineStr">
+        <is>
+          <t>16321.97137</t>
+        </is>
+      </c>
       <c r="E14" s="6" t="n"/>
     </row>
     <row r="15">
@@ -764,7 +804,11 @@
         <v>650000</v>
       </c>
       <c r="C15" s="11" t="n"/>
-      <c r="D15" s="11" t="n"/>
+      <c r="D15" s="11" t="inlineStr">
+        <is>
+          <t>19550.50262</t>
+        </is>
+      </c>
       <c r="E15" s="6" t="n"/>
     </row>
     <row r="16">
@@ -775,7 +819,11 @@
         <v>700000</v>
       </c>
       <c r="C16" s="11" t="n"/>
-      <c r="D16" s="11" t="n"/>
+      <c r="D16" s="11" t="inlineStr">
+        <is>
+          <t>24435.47438</t>
+        </is>
+      </c>
       <c r="E16" s="6" t="n"/>
     </row>
     <row r="17">
@@ -786,7 +834,11 @@
         <v>750000</v>
       </c>
       <c r="C17" s="11" t="n"/>
-      <c r="D17" s="11" t="n"/>
+      <c r="D17" s="11" t="inlineStr">
+        <is>
+          <t>25468.59240</t>
+        </is>
+      </c>
       <c r="E17" s="6" t="n"/>
     </row>
     <row r="18">
@@ -797,7 +849,11 @@
         <v>800000</v>
       </c>
       <c r="C18" s="11" t="n"/>
-      <c r="D18" s="11" t="n"/>
+      <c r="D18" s="11" t="inlineStr">
+        <is>
+          <t>29850.17472</t>
+        </is>
+      </c>
       <c r="E18" s="6" t="n"/>
     </row>
     <row r="19">

</xml_diff>